<commit_message>
TextBlob NaiveBayes added - Folder Restructure
</commit_message>
<xml_diff>
--- a/Datasets/Calculation Result/Classification Report/Classification Report 0.5TH - 0.3TH -0.1TH comparison.xlsx
+++ b/Datasets/Calculation Result/Classification Report/Classification Report 0.5TH - 0.3TH -0.1TH comparison.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\QuangDaoVuNgoc\github\bachelorthesis\Datasets\Calculation Result\Classification Report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02F3FC38-1912-4BB7-B55F-232D0B4E48C8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93BE7AB7-4906-4B48-B004-29F900A77251}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3510" yWindow="3510" windowWidth="20910" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="390" yWindow="0" windowWidth="27870" windowHeight="16200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -387,10 +387,10 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -673,8 +673,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:W46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="P11" sqref="P11"/>
+    <sheetView tabSelected="1" topLeftCell="H13" workbookViewId="0">
+      <selection activeCell="K48" sqref="K48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -736,10 +736,10 @@
       <c r="D3" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="4"/>
+      <c r="F3" s="5"/>
       <c r="G3" s="1" t="s">
         <v>6</v>
       </c>
@@ -755,10 +755,10 @@
       <c r="L3" t="s">
         <v>4</v>
       </c>
-      <c r="M3" s="4" t="s">
+      <c r="M3" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="N3" s="4"/>
+      <c r="N3" s="5"/>
       <c r="O3" s="1" t="s">
         <v>6</v>
       </c>
@@ -774,10 +774,10 @@
       <c r="T3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="U3" s="4" t="s">
+      <c r="U3" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="V3" s="4"/>
+      <c r="V3" s="5"/>
       <c r="W3" s="1" t="s">
         <v>6</v>
       </c>
@@ -793,10 +793,10 @@
       <c r="D4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E4" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F4" s="4"/>
+      <c r="F4" s="5"/>
       <c r="G4" s="1">
         <v>504</v>
       </c>
@@ -810,10 +810,10 @@
       <c r="L4" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="M4" s="4" t="s">
+      <c r="M4" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="N4" s="4"/>
+      <c r="N4" s="5"/>
       <c r="O4" s="1">
         <v>504</v>
       </c>
@@ -827,10 +827,10 @@
       <c r="T4" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="U4" s="4" t="s">
+      <c r="U4" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="V4" s="4"/>
+      <c r="V4" s="5"/>
       <c r="W4" s="1">
         <v>504</v>
       </c>
@@ -846,10 +846,10 @@
       <c r="D5" t="s">
         <v>13</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="E5" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F5" s="4"/>
+      <c r="F5" s="5"/>
       <c r="G5" s="1">
         <v>496</v>
       </c>
@@ -863,10 +863,10 @@
       <c r="L5" t="s">
         <v>49</v>
       </c>
-      <c r="M5" s="4" t="s">
+      <c r="M5" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="N5" s="4"/>
+      <c r="N5" s="5"/>
       <c r="O5" s="1">
         <v>496</v>
       </c>
@@ -880,10 +880,10 @@
       <c r="T5" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="U5" s="4" t="s">
+      <c r="U5" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="V5" s="4"/>
+      <c r="V5" s="5"/>
       <c r="W5" s="1">
         <v>496</v>
       </c>
@@ -899,10 +899,10 @@
       <c r="D6" t="s">
         <v>16</v>
       </c>
-      <c r="E6" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="F6" s="4"/>
+      <c r="E6" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F6" s="5"/>
       <c r="G6" s="1">
         <v>504</v>
       </c>
@@ -916,10 +916,10 @@
       <c r="L6" t="s">
         <v>16</v>
       </c>
-      <c r="M6" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="N6" s="4"/>
+      <c r="M6" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="N6" s="5"/>
       <c r="O6" s="1">
         <v>504</v>
       </c>
@@ -933,10 +933,10 @@
       <c r="T6" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="U6" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="V6" s="4"/>
+      <c r="U6" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="V6" s="5"/>
       <c r="W6" s="1">
         <v>504</v>
       </c>
@@ -963,10 +963,10 @@
       <c r="B8" t="s">
         <v>17</v>
       </c>
-      <c r="E8" s="4" t="s">
+      <c r="E8" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="F8" s="4"/>
+      <c r="F8" s="5"/>
       <c r="G8" s="1">
         <v>1000</v>
       </c>
@@ -974,10 +974,10 @@
       <c r="J8" t="s">
         <v>17</v>
       </c>
-      <c r="M8" s="4" t="s">
+      <c r="M8" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="N8" s="4"/>
+      <c r="N8" s="5"/>
       <c r="O8" s="1">
         <v>1000</v>
       </c>
@@ -987,10 +987,10 @@
       </c>
       <c r="S8" s="2"/>
       <c r="T8" s="2"/>
-      <c r="U8" s="4" t="s">
+      <c r="U8" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="V8" s="4"/>
+      <c r="V8" s="5"/>
       <c r="W8" s="1">
         <v>1000</v>
       </c>
@@ -1006,10 +1006,10 @@
       <c r="D9" t="s">
         <v>21</v>
       </c>
-      <c r="E9" s="4" t="s">
+      <c r="E9" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="F9" s="4"/>
+      <c r="F9" s="5"/>
       <c r="G9" s="1">
         <v>1000</v>
       </c>
@@ -1023,10 +1023,10 @@
       <c r="L9" t="s">
         <v>74</v>
       </c>
-      <c r="M9" s="4" t="s">
+      <c r="M9" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="N9" s="4"/>
+      <c r="N9" s="5"/>
       <c r="O9" s="1">
         <v>1000</v>
       </c>
@@ -1040,10 +1040,10 @@
       <c r="T9" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="U9" s="4" t="s">
+      <c r="U9" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="V9" s="4"/>
+      <c r="V9" s="5"/>
       <c r="W9" s="1">
         <v>1000</v>
       </c>
@@ -1059,10 +1059,10 @@
       <c r="D10" t="s">
         <v>18</v>
       </c>
-      <c r="E10" s="4" t="s">
+      <c r="E10" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="F10" s="4"/>
+      <c r="F10" s="5"/>
       <c r="G10" s="1">
         <v>1000</v>
       </c>
@@ -1076,10 +1076,10 @@
       <c r="L10" t="s">
         <v>10</v>
       </c>
-      <c r="M10" s="4" t="s">
+      <c r="M10" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="N10" s="4"/>
+      <c r="N10" s="5"/>
       <c r="O10" s="1">
         <v>1000</v>
       </c>
@@ -1093,10 +1093,10 @@
       <c r="T10" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="U10" s="4" t="s">
+      <c r="U10" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="V10" s="4"/>
+      <c r="V10" s="5"/>
       <c r="W10" s="1">
         <v>1000</v>
       </c>
@@ -1123,10 +1123,10 @@
       <c r="D12" t="s">
         <v>4</v>
       </c>
-      <c r="E12" s="4" t="s">
+      <c r="E12" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="F12" s="4"/>
+      <c r="F12" s="5"/>
       <c r="G12" s="1" t="s">
         <v>6</v>
       </c>
@@ -1142,10 +1142,10 @@
       <c r="L12" t="s">
         <v>4</v>
       </c>
-      <c r="M12" s="4" t="s">
+      <c r="M12" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="N12" s="4"/>
+      <c r="N12" s="5"/>
       <c r="O12" s="1" t="s">
         <v>6</v>
       </c>
@@ -1161,10 +1161,10 @@
       <c r="T12" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="U12" s="4" t="s">
+      <c r="U12" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="V12" s="4"/>
+      <c r="V12" s="5"/>
       <c r="W12" s="1" t="s">
         <v>6</v>
       </c>
@@ -1180,10 +1180,10 @@
       <c r="D13" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="E13" s="4" t="s">
+      <c r="E13" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="F13" s="4"/>
+      <c r="F13" s="5"/>
       <c r="G13" s="1">
         <v>498</v>
       </c>
@@ -1197,10 +1197,10 @@
       <c r="L13" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="M13" s="4" t="s">
+      <c r="M13" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="N13" s="4"/>
+      <c r="N13" s="5"/>
       <c r="O13" s="1">
         <v>498</v>
       </c>
@@ -1214,10 +1214,10 @@
       <c r="T13" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="U13" s="4" t="s">
+      <c r="U13" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="V13" s="4"/>
+      <c r="V13" s="5"/>
       <c r="W13" s="1">
         <v>498</v>
       </c>
@@ -1233,10 +1233,10 @@
       <c r="D14" t="s">
         <v>28</v>
       </c>
-      <c r="E14" s="4" t="s">
+      <c r="E14" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="F14" s="4"/>
+      <c r="F14" s="5"/>
       <c r="G14" s="1">
         <v>498</v>
       </c>
@@ -1250,10 +1250,10 @@
       <c r="L14" t="s">
         <v>13</v>
       </c>
-      <c r="M14" s="4" t="s">
+      <c r="M14" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="N14" s="4"/>
+      <c r="N14" s="5"/>
       <c r="O14" s="1">
         <v>498</v>
       </c>
@@ -1267,10 +1267,10 @@
       <c r="T14" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="U14" s="4" t="s">
+      <c r="U14" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="V14" s="4"/>
+      <c r="V14" s="5"/>
       <c r="W14" s="1">
         <v>498</v>
       </c>
@@ -1286,10 +1286,10 @@
       <c r="D15" t="s">
         <v>16</v>
       </c>
-      <c r="E15" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="F15" s="4"/>
+      <c r="E15" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F15" s="5"/>
       <c r="G15" s="1">
         <v>0</v>
       </c>
@@ -1303,10 +1303,10 @@
       <c r="L15" t="s">
         <v>16</v>
       </c>
-      <c r="M15" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="N15" s="4"/>
+      <c r="M15" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="N15" s="5"/>
       <c r="O15" s="1">
         <v>0</v>
       </c>
@@ -1320,10 +1320,10 @@
       <c r="T15" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="U15" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="V15" s="4"/>
+      <c r="U15" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="V15" s="5"/>
       <c r="W15" s="1">
         <v>0</v>
       </c>
@@ -1350,10 +1350,10 @@
       <c r="B17" t="s">
         <v>17</v>
       </c>
-      <c r="E17" s="4" t="s">
+      <c r="E17" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="F17" s="4"/>
+      <c r="F17" s="5"/>
       <c r="G17" s="1">
         <v>996</v>
       </c>
@@ -1361,10 +1361,10 @@
       <c r="J17" t="s">
         <v>17</v>
       </c>
-      <c r="M17" s="4" t="s">
+      <c r="M17" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="N17" s="4"/>
+      <c r="N17" s="5"/>
       <c r="O17" s="1">
         <v>996</v>
       </c>
@@ -1374,10 +1374,10 @@
       </c>
       <c r="S17" s="2"/>
       <c r="T17" s="2"/>
-      <c r="U17" s="4" t="s">
+      <c r="U17" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="V17" s="4"/>
+      <c r="V17" s="5"/>
       <c r="W17" s="1">
         <v>996</v>
       </c>
@@ -1393,10 +1393,10 @@
       <c r="D18" t="s">
         <v>29</v>
       </c>
-      <c r="E18" s="4" t="s">
+      <c r="E18" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="F18" s="4"/>
+      <c r="F18" s="5"/>
       <c r="G18" s="1">
         <v>996</v>
       </c>
@@ -1410,10 +1410,10 @@
       <c r="L18" t="s">
         <v>18</v>
       </c>
-      <c r="M18" s="4" t="s">
+      <c r="M18" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="N18" s="4"/>
+      <c r="N18" s="5"/>
       <c r="O18" s="1">
         <v>996</v>
       </c>
@@ -1427,10 +1427,10 @@
       <c r="T18" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="U18" s="4" t="s">
+      <c r="U18" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="V18" s="4"/>
+      <c r="V18" s="5"/>
       <c r="W18" s="1">
         <v>996</v>
       </c>
@@ -1446,10 +1446,10 @@
       <c r="D19" t="s">
         <v>13</v>
       </c>
-      <c r="E19" s="4" t="s">
+      <c r="E19" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="F19" s="4"/>
+      <c r="F19" s="5"/>
       <c r="G19" s="1">
         <v>996</v>
       </c>
@@ -1463,10 +1463,10 @@
       <c r="L19" t="s">
         <v>46</v>
       </c>
-      <c r="M19" s="4" t="s">
+      <c r="M19" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="N19" s="4"/>
+      <c r="N19" s="5"/>
       <c r="O19" s="1">
         <v>996</v>
       </c>
@@ -1480,10 +1480,10 @@
       <c r="T19" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="U19" s="4" t="s">
+      <c r="U19" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="V19" s="4"/>
+      <c r="V19" s="5"/>
       <c r="W19" s="1">
         <v>996</v>
       </c>
@@ -1510,10 +1510,10 @@
       <c r="D21" t="s">
         <v>4</v>
       </c>
-      <c r="E21" s="4" t="s">
+      <c r="E21" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="F21" s="4"/>
+      <c r="F21" s="5"/>
       <c r="G21" s="1" t="s">
         <v>6</v>
       </c>
@@ -1529,10 +1529,10 @@
       <c r="L21" t="s">
         <v>4</v>
       </c>
-      <c r="M21" s="4" t="s">
+      <c r="M21" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="N21" s="4"/>
+      <c r="N21" s="5"/>
       <c r="O21" s="1" t="s">
         <v>6</v>
       </c>
@@ -1548,10 +1548,10 @@
       <c r="T21" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="U21" s="4" t="s">
+      <c r="U21" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="V21" s="4"/>
+      <c r="V21" s="5"/>
       <c r="W21" s="1" t="s">
         <v>6</v>
       </c>
@@ -1567,10 +1567,10 @@
       <c r="D22" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="E22" s="4" t="s">
+      <c r="E22" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="F22" s="4"/>
+      <c r="F22" s="5"/>
       <c r="G22" s="1">
         <v>500</v>
       </c>
@@ -1584,10 +1584,10 @@
       <c r="L22" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="M22" s="4" t="s">
+      <c r="M22" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="N22" s="4"/>
+      <c r="N22" s="5"/>
       <c r="O22" s="1">
         <v>500</v>
       </c>
@@ -1601,10 +1601,10 @@
       <c r="T22" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="U22" s="4" t="s">
+      <c r="U22" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="V22" s="4"/>
+      <c r="V22" s="5"/>
       <c r="W22" s="1">
         <v>500</v>
       </c>
@@ -1620,10 +1620,10 @@
       <c r="D23" t="s">
         <v>37</v>
       </c>
-      <c r="E23" s="4" t="s">
+      <c r="E23" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="F23" s="4"/>
+      <c r="F23" s="5"/>
       <c r="G23" s="1">
         <v>500</v>
       </c>
@@ -1637,10 +1637,10 @@
       <c r="L23" t="s">
         <v>60</v>
       </c>
-      <c r="M23" s="4" t="s">
+      <c r="M23" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="N23" s="4"/>
+      <c r="N23" s="5"/>
       <c r="O23" s="1">
         <v>500</v>
       </c>
@@ -1654,10 +1654,10 @@
       <c r="T23" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="U23" s="4" t="s">
+      <c r="U23" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="V23" s="4"/>
+      <c r="V23" s="5"/>
       <c r="W23" s="1">
         <v>500</v>
       </c>
@@ -1673,10 +1673,10 @@
       <c r="D24" t="s">
         <v>16</v>
       </c>
-      <c r="E24" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="F24" s="4"/>
+      <c r="E24" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F24" s="5"/>
       <c r="G24" s="1"/>
       <c r="I24" s="3"/>
       <c r="J24" t="s">
@@ -1688,10 +1688,10 @@
       <c r="L24" t="s">
         <v>16</v>
       </c>
-      <c r="M24" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="N24" s="4"/>
+      <c r="M24" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="N24" s="5"/>
       <c r="O24" s="1"/>
       <c r="Q24" s="3"/>
       <c r="R24" s="2" t="s">
@@ -1703,10 +1703,10 @@
       <c r="T24" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="U24" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="V24" s="4"/>
+      <c r="U24" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="V24" s="5"/>
       <c r="W24" s="1"/>
     </row>
     <row r="25" spans="1:23" x14ac:dyDescent="0.25">
@@ -1731,10 +1731,10 @@
       <c r="B26" t="s">
         <v>17</v>
       </c>
-      <c r="E26" s="4" t="s">
+      <c r="E26" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="F26" s="4"/>
+      <c r="F26" s="5"/>
       <c r="G26" s="1">
         <v>1000</v>
       </c>
@@ -1742,10 +1742,10 @@
       <c r="J26" t="s">
         <v>17</v>
       </c>
-      <c r="M26" s="4" t="s">
+      <c r="M26" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="N26" s="4"/>
+      <c r="N26" s="5"/>
       <c r="O26" s="1">
         <v>1000</v>
       </c>
@@ -1755,10 +1755,10 @@
       </c>
       <c r="S26" s="2"/>
       <c r="T26" s="2"/>
-      <c r="U26" s="4" t="s">
+      <c r="U26" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="V26" s="4"/>
+      <c r="V26" s="5"/>
       <c r="W26" s="1">
         <v>1000</v>
       </c>
@@ -1774,10 +1774,10 @@
       <c r="D27" t="s">
         <v>41</v>
       </c>
-      <c r="E27" s="4" t="s">
+      <c r="E27" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="F27" s="4"/>
+      <c r="F27" s="5"/>
       <c r="G27" s="1">
         <v>1000</v>
       </c>
@@ -1791,10 +1791,10 @@
       <c r="L27" t="s">
         <v>78</v>
       </c>
-      <c r="M27" s="4" t="s">
+      <c r="M27" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="N27" s="4"/>
+      <c r="N27" s="5"/>
       <c r="O27" s="1">
         <v>1000</v>
       </c>
@@ -1808,10 +1808,10 @@
       <c r="T27" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="U27" s="4" t="s">
+      <c r="U27" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="V27" s="4"/>
+      <c r="V27" s="5"/>
       <c r="W27" s="1">
         <v>1000</v>
       </c>
@@ -1827,10 +1827,10 @@
       <c r="D28" t="s">
         <v>39</v>
       </c>
-      <c r="E28" s="4" t="s">
+      <c r="E28" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="F28" s="4"/>
+      <c r="F28" s="5"/>
       <c r="G28" s="1">
         <v>1000</v>
       </c>
@@ -1844,10 +1844,10 @@
       <c r="L28" t="s">
         <v>76</v>
       </c>
-      <c r="M28" s="4" t="s">
+      <c r="M28" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="N28" s="4"/>
+      <c r="N28" s="5"/>
       <c r="O28" s="1">
         <v>1000</v>
       </c>
@@ -1861,10 +1861,10 @@
       <c r="T28" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="U28" s="4" t="s">
+      <c r="U28" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="V28" s="4"/>
+      <c r="V28" s="5"/>
       <c r="W28" s="1">
         <v>1000</v>
       </c>
@@ -1891,10 +1891,10 @@
       <c r="D30" t="s">
         <v>4</v>
       </c>
-      <c r="E30" s="5" t="s">
+      <c r="E30" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F30" s="5"/>
+      <c r="F30" s="4"/>
       <c r="G30" s="1" t="s">
         <v>6</v>
       </c>
@@ -1910,10 +1910,10 @@
       <c r="L30" t="s">
         <v>4</v>
       </c>
-      <c r="M30" s="5" t="s">
+      <c r="M30" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="N30" s="5"/>
+      <c r="N30" s="4"/>
       <c r="O30" s="1" t="s">
         <v>6</v>
       </c>
@@ -1929,10 +1929,10 @@
       <c r="T30" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="U30" s="5" t="s">
+      <c r="U30" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="V30" s="5"/>
+      <c r="V30" s="4"/>
       <c r="W30" s="1" t="s">
         <v>6</v>
       </c>
@@ -1948,10 +1948,10 @@
       <c r="D31" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="E31" s="4" t="s">
+      <c r="E31" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="F31" s="4"/>
+      <c r="F31" s="5"/>
       <c r="G31">
         <v>167</v>
       </c>
@@ -1965,10 +1965,10 @@
       <c r="L31" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="M31" s="4" t="s">
+      <c r="M31" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="N31" s="4"/>
+      <c r="N31" s="5"/>
       <c r="O31">
         <v>167</v>
       </c>
@@ -1982,10 +1982,10 @@
       <c r="T31" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="U31" s="4" t="s">
+      <c r="U31" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="V31" s="4"/>
+      <c r="V31" s="5"/>
       <c r="W31" s="2">
         <v>167</v>
       </c>
@@ -2001,10 +2001,10 @@
       <c r="D32" t="s">
         <v>27</v>
       </c>
-      <c r="E32" s="4" t="s">
+      <c r="E32" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="F32" s="4"/>
+      <c r="F32" s="5"/>
       <c r="G32">
         <v>769</v>
       </c>
@@ -2018,10 +2018,10 @@
       <c r="L32" t="s">
         <v>18</v>
       </c>
-      <c r="M32" s="4" t="s">
+      <c r="M32" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="N32" s="4"/>
+      <c r="N32" s="5"/>
       <c r="O32">
         <v>769</v>
       </c>
@@ -2035,10 +2035,10 @@
       <c r="T32" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="U32" s="4" t="s">
+      <c r="U32" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="V32" s="4"/>
+      <c r="V32" s="5"/>
       <c r="W32" s="2">
         <v>769</v>
       </c>
@@ -2054,10 +2054,10 @@
       <c r="D33" t="s">
         <v>16</v>
       </c>
-      <c r="E33" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="F33" s="4"/>
+      <c r="E33" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F33" s="5"/>
       <c r="G33">
         <v>0</v>
       </c>
@@ -2071,10 +2071,10 @@
       <c r="L33" t="s">
         <v>16</v>
       </c>
-      <c r="M33" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="N33" s="4"/>
+      <c r="M33" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="N33" s="5"/>
       <c r="O33">
         <v>0</v>
       </c>
@@ -2088,10 +2088,10 @@
       <c r="T33" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="U33" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="V33" s="4"/>
+      <c r="U33" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="V33" s="5"/>
       <c r="W33" s="2">
         <v>0</v>
       </c>
@@ -2116,10 +2116,10 @@
       <c r="B35" t="s">
         <v>17</v>
       </c>
-      <c r="E35" s="4" t="s">
+      <c r="E35" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F35" s="4"/>
+      <c r="F35" s="5"/>
       <c r="G35">
         <v>936</v>
       </c>
@@ -2127,10 +2127,10 @@
       <c r="J35" t="s">
         <v>17</v>
       </c>
-      <c r="M35" s="4" t="s">
+      <c r="M35" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="N35" s="4"/>
+      <c r="N35" s="5"/>
       <c r="O35">
         <v>936</v>
       </c>
@@ -2140,10 +2140,10 @@
       </c>
       <c r="S35" s="2"/>
       <c r="T35" s="2"/>
-      <c r="U35" s="4" t="s">
+      <c r="U35" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="V35" s="4"/>
+      <c r="V35" s="5"/>
       <c r="W35" s="2">
         <v>936</v>
       </c>
@@ -2159,10 +2159,10 @@
       <c r="D36" t="s">
         <v>21</v>
       </c>
-      <c r="E36" s="4" t="s">
+      <c r="E36" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="F36" s="4"/>
+      <c r="F36" s="5"/>
       <c r="G36">
         <v>936</v>
       </c>
@@ -2176,10 +2176,10 @@
       <c r="L36" t="s">
         <v>74</v>
       </c>
-      <c r="M36" s="4" t="s">
+      <c r="M36" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="N36" s="4"/>
+      <c r="N36" s="5"/>
       <c r="O36">
         <v>936</v>
       </c>
@@ -2193,10 +2193,10 @@
       <c r="T36" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="U36" s="4" t="s">
+      <c r="U36" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="V36" s="4"/>
+      <c r="V36" s="5"/>
       <c r="W36" s="2">
         <v>936</v>
       </c>
@@ -2212,10 +2212,10 @@
       <c r="D37" t="s">
         <v>14</v>
       </c>
-      <c r="E37" s="4" t="s">
+      <c r="E37" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="F37" s="4"/>
+      <c r="F37" s="5"/>
       <c r="G37">
         <v>936</v>
       </c>
@@ -2229,10 +2229,10 @@
       <c r="L37" t="s">
         <v>9</v>
       </c>
-      <c r="M37" s="4" t="s">
+      <c r="M37" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="N37" s="4"/>
+      <c r="N37" s="5"/>
       <c r="O37">
         <v>936</v>
       </c>
@@ -2246,10 +2246,10 @@
       <c r="T37" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="U37" s="4" t="s">
+      <c r="U37" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="V37" s="4"/>
+      <c r="V37" s="5"/>
       <c r="W37" s="2">
         <v>936</v>
       </c>
@@ -2276,10 +2276,10 @@
       <c r="D39" t="s">
         <v>4</v>
       </c>
-      <c r="E39" s="4" t="s">
+      <c r="E39" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="F39" s="4"/>
+      <c r="F39" s="5"/>
       <c r="G39" s="1" t="s">
         <v>6</v>
       </c>
@@ -2295,10 +2295,10 @@
       <c r="L39" t="s">
         <v>4</v>
       </c>
-      <c r="M39" s="4" t="s">
+      <c r="M39" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="N39" s="4"/>
+      <c r="N39" s="5"/>
       <c r="O39" s="1" t="s">
         <v>6</v>
       </c>
@@ -2314,10 +2314,10 @@
       <c r="T39" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="U39" s="4" t="s">
+      <c r="U39" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="V39" s="4"/>
+      <c r="V39" s="5"/>
       <c r="W39" s="1" t="s">
         <v>6</v>
       </c>
@@ -2333,10 +2333,10 @@
       <c r="D40" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="E40" s="4" t="s">
+      <c r="E40" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="F40" s="4"/>
+      <c r="F40" s="5"/>
       <c r="G40" s="1">
         <v>483</v>
       </c>
@@ -2348,12 +2348,12 @@
         <v>36</v>
       </c>
       <c r="L40" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="M40" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="M40" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="N40" s="4"/>
+      <c r="N40" s="5"/>
       <c r="O40" s="1">
         <v>483</v>
       </c>
@@ -2367,10 +2367,10 @@
       <c r="T40" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="U40" s="4" t="s">
+      <c r="U40" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="V40" s="4"/>
+      <c r="V40" s="5"/>
       <c r="W40" s="1">
         <v>483</v>
       </c>
@@ -2386,10 +2386,10 @@
       <c r="D41" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E41" s="4" t="s">
+      <c r="E41" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F41" s="4"/>
+      <c r="F41" s="5"/>
       <c r="G41" s="1">
         <v>517</v>
       </c>
@@ -2403,10 +2403,10 @@
       <c r="L41" t="s">
         <v>18</v>
       </c>
-      <c r="M41" s="4" t="s">
+      <c r="M41" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="N41" s="4"/>
+      <c r="N41" s="5"/>
       <c r="O41" s="1">
         <v>517</v>
       </c>
@@ -2420,10 +2420,10 @@
       <c r="T41" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="U41" s="4" t="s">
+      <c r="U41" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="V41" s="4"/>
+      <c r="V41" s="5"/>
       <c r="W41" s="1">
         <v>517</v>
       </c>
@@ -2439,10 +2439,10 @@
       <c r="D42" t="s">
         <v>16</v>
       </c>
-      <c r="E42" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="F42" s="4"/>
+      <c r="E42" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F42" s="5"/>
       <c r="G42" s="1">
         <v>0</v>
       </c>
@@ -2456,10 +2456,10 @@
       <c r="L42" t="s">
         <v>16</v>
       </c>
-      <c r="M42" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="N42" s="4"/>
+      <c r="M42" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="N42" s="5"/>
       <c r="O42" s="1">
         <v>0</v>
       </c>
@@ -2473,10 +2473,10 @@
       <c r="T42" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="U42" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="V42" s="4"/>
+      <c r="U42" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="V42" s="5"/>
       <c r="W42" s="1">
         <v>0</v>
       </c>
@@ -2503,10 +2503,10 @@
       <c r="B44" t="s">
         <v>17</v>
       </c>
-      <c r="E44" s="4" t="s">
+      <c r="E44" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="F44" s="4"/>
+      <c r="F44" s="5"/>
       <c r="G44" s="1">
         <v>1000</v>
       </c>
@@ -2514,10 +2514,10 @@
       <c r="J44" t="s">
         <v>17</v>
       </c>
-      <c r="M44" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="N44" s="4"/>
+      <c r="M44" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="N44" s="5"/>
       <c r="O44" s="1">
         <v>1000</v>
       </c>
@@ -2527,10 +2527,10 @@
       </c>
       <c r="S44" s="2"/>
       <c r="T44" s="2"/>
-      <c r="U44" s="4" t="s">
+      <c r="U44" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="V44" s="4"/>
+      <c r="V44" s="5"/>
       <c r="W44" s="1">
         <v>1000</v>
       </c>
@@ -2546,10 +2546,10 @@
       <c r="D45" t="s">
         <v>14</v>
       </c>
-      <c r="E45" s="4" t="s">
+      <c r="E45" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="F45" s="4"/>
+      <c r="F45" s="5"/>
       <c r="G45" s="1">
         <v>1000</v>
       </c>
@@ -2563,10 +2563,10 @@
       <c r="L45" t="s">
         <v>83</v>
       </c>
-      <c r="M45" s="4" t="s">
+      <c r="M45" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="N45" s="4"/>
+      <c r="N45" s="5"/>
       <c r="O45" s="1">
         <v>1000</v>
       </c>
@@ -2580,10 +2580,10 @@
       <c r="T45" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="U45" s="4" t="s">
+      <c r="U45" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="V45" s="4"/>
+      <c r="V45" s="5"/>
       <c r="W45" s="1">
         <v>1000</v>
       </c>
@@ -2599,10 +2599,10 @@
       <c r="D46" t="s">
         <v>49</v>
       </c>
-      <c r="E46" s="4" t="s">
+      <c r="E46" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="F46" s="4"/>
+      <c r="F46" s="5"/>
       <c r="G46" s="1">
         <v>1000</v>
       </c>
@@ -2616,10 +2616,10 @@
       <c r="L46" t="s">
         <v>81</v>
       </c>
-      <c r="M46" s="4" t="s">
+      <c r="M46" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="N46" s="4"/>
+      <c r="N46" s="5"/>
       <c r="O46" s="1">
         <v>1000</v>
       </c>
@@ -2633,16 +2633,123 @@
       <c r="T46" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="U46" s="4" t="s">
+      <c r="U46" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="V46" s="4"/>
+      <c r="V46" s="5"/>
       <c r="W46" s="1">
         <v>1000</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="123">
+    <mergeCell ref="Q39:Q46"/>
+    <mergeCell ref="U39:V39"/>
+    <mergeCell ref="U40:V40"/>
+    <mergeCell ref="U41:V41"/>
+    <mergeCell ref="U42:V42"/>
+    <mergeCell ref="U44:V44"/>
+    <mergeCell ref="U45:V45"/>
+    <mergeCell ref="U46:V46"/>
+    <mergeCell ref="Q30:Q37"/>
+    <mergeCell ref="U30:V30"/>
+    <mergeCell ref="U31:V31"/>
+    <mergeCell ref="U32:V32"/>
+    <mergeCell ref="U33:V33"/>
+    <mergeCell ref="U35:V35"/>
+    <mergeCell ref="U36:V36"/>
+    <mergeCell ref="U37:V37"/>
+    <mergeCell ref="Q21:Q28"/>
+    <mergeCell ref="U21:V21"/>
+    <mergeCell ref="U22:V22"/>
+    <mergeCell ref="U23:V23"/>
+    <mergeCell ref="U24:V24"/>
+    <mergeCell ref="U26:V26"/>
+    <mergeCell ref="U27:V27"/>
+    <mergeCell ref="U28:V28"/>
+    <mergeCell ref="Q12:Q19"/>
+    <mergeCell ref="U12:V12"/>
+    <mergeCell ref="U13:V13"/>
+    <mergeCell ref="U14:V14"/>
+    <mergeCell ref="U15:V15"/>
+    <mergeCell ref="U17:V17"/>
+    <mergeCell ref="U18:V18"/>
+    <mergeCell ref="U19:V19"/>
+    <mergeCell ref="R1:V2"/>
+    <mergeCell ref="Q3:Q10"/>
+    <mergeCell ref="U3:V3"/>
+    <mergeCell ref="U4:V4"/>
+    <mergeCell ref="U5:V5"/>
+    <mergeCell ref="U6:V6"/>
+    <mergeCell ref="U8:V8"/>
+    <mergeCell ref="U9:V9"/>
+    <mergeCell ref="U10:V10"/>
+    <mergeCell ref="B1:F2"/>
+    <mergeCell ref="A3:A10"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="A12:A19"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="A21:A28"/>
+    <mergeCell ref="E21:F21"/>
+    <mergeCell ref="E22:F22"/>
+    <mergeCell ref="E23:F23"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="E27:F27"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="A30:A37"/>
+    <mergeCell ref="E30:F30"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="A39:A46"/>
+    <mergeCell ref="E39:F39"/>
+    <mergeCell ref="E40:F40"/>
+    <mergeCell ref="E41:F41"/>
+    <mergeCell ref="E42:F42"/>
+    <mergeCell ref="E44:F44"/>
+    <mergeCell ref="E45:F45"/>
+    <mergeCell ref="E46:F46"/>
+    <mergeCell ref="J1:N2"/>
+    <mergeCell ref="I3:I10"/>
+    <mergeCell ref="M3:N3"/>
+    <mergeCell ref="M4:N4"/>
+    <mergeCell ref="M5:N5"/>
+    <mergeCell ref="M6:N6"/>
+    <mergeCell ref="M8:N8"/>
+    <mergeCell ref="M9:N9"/>
+    <mergeCell ref="M10:N10"/>
+    <mergeCell ref="I12:I19"/>
+    <mergeCell ref="M12:N12"/>
+    <mergeCell ref="M13:N13"/>
+    <mergeCell ref="M14:N14"/>
+    <mergeCell ref="M15:N15"/>
+    <mergeCell ref="M17:N17"/>
+    <mergeCell ref="M18:N18"/>
+    <mergeCell ref="M19:N19"/>
+    <mergeCell ref="I21:I28"/>
+    <mergeCell ref="M21:N21"/>
+    <mergeCell ref="M22:N22"/>
+    <mergeCell ref="M23:N23"/>
+    <mergeCell ref="M24:N24"/>
+    <mergeCell ref="M26:N26"/>
+    <mergeCell ref="M27:N27"/>
+    <mergeCell ref="M28:N28"/>
     <mergeCell ref="I30:I37"/>
     <mergeCell ref="M30:N30"/>
     <mergeCell ref="M31:N31"/>
@@ -2659,113 +2766,6 @@
     <mergeCell ref="M44:N44"/>
     <mergeCell ref="M45:N45"/>
     <mergeCell ref="M46:N46"/>
-    <mergeCell ref="I12:I19"/>
-    <mergeCell ref="M12:N12"/>
-    <mergeCell ref="M13:N13"/>
-    <mergeCell ref="M14:N14"/>
-    <mergeCell ref="M15:N15"/>
-    <mergeCell ref="M17:N17"/>
-    <mergeCell ref="M18:N18"/>
-    <mergeCell ref="M19:N19"/>
-    <mergeCell ref="I21:I28"/>
-    <mergeCell ref="M21:N21"/>
-    <mergeCell ref="M22:N22"/>
-    <mergeCell ref="M23:N23"/>
-    <mergeCell ref="M24:N24"/>
-    <mergeCell ref="M26:N26"/>
-    <mergeCell ref="M27:N27"/>
-    <mergeCell ref="M28:N28"/>
-    <mergeCell ref="J1:N2"/>
-    <mergeCell ref="I3:I10"/>
-    <mergeCell ref="M3:N3"/>
-    <mergeCell ref="M4:N4"/>
-    <mergeCell ref="M5:N5"/>
-    <mergeCell ref="M6:N6"/>
-    <mergeCell ref="M8:N8"/>
-    <mergeCell ref="M9:N9"/>
-    <mergeCell ref="M10:N10"/>
-    <mergeCell ref="A30:A37"/>
-    <mergeCell ref="E30:F30"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="A39:A46"/>
-    <mergeCell ref="E39:F39"/>
-    <mergeCell ref="E40:F40"/>
-    <mergeCell ref="E41:F41"/>
-    <mergeCell ref="E42:F42"/>
-    <mergeCell ref="E44:F44"/>
-    <mergeCell ref="E45:F45"/>
-    <mergeCell ref="E46:F46"/>
-    <mergeCell ref="A12:A19"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="E17:F17"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="E19:F19"/>
-    <mergeCell ref="A21:A28"/>
-    <mergeCell ref="E21:F21"/>
-    <mergeCell ref="E22:F22"/>
-    <mergeCell ref="E23:F23"/>
-    <mergeCell ref="E24:F24"/>
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="E27:F27"/>
-    <mergeCell ref="E28:F28"/>
-    <mergeCell ref="B1:F2"/>
-    <mergeCell ref="A3:A10"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="R1:V2"/>
-    <mergeCell ref="Q3:Q10"/>
-    <mergeCell ref="U3:V3"/>
-    <mergeCell ref="U4:V4"/>
-    <mergeCell ref="U5:V5"/>
-    <mergeCell ref="U6:V6"/>
-    <mergeCell ref="U8:V8"/>
-    <mergeCell ref="U9:V9"/>
-    <mergeCell ref="U10:V10"/>
-    <mergeCell ref="Q21:Q28"/>
-    <mergeCell ref="U21:V21"/>
-    <mergeCell ref="U22:V22"/>
-    <mergeCell ref="U23:V23"/>
-    <mergeCell ref="U24:V24"/>
-    <mergeCell ref="U26:V26"/>
-    <mergeCell ref="U27:V27"/>
-    <mergeCell ref="U28:V28"/>
-    <mergeCell ref="Q12:Q19"/>
-    <mergeCell ref="U12:V12"/>
-    <mergeCell ref="U13:V13"/>
-    <mergeCell ref="U14:V14"/>
-    <mergeCell ref="U15:V15"/>
-    <mergeCell ref="U17:V17"/>
-    <mergeCell ref="U18:V18"/>
-    <mergeCell ref="U19:V19"/>
-    <mergeCell ref="Q39:Q46"/>
-    <mergeCell ref="U39:V39"/>
-    <mergeCell ref="U40:V40"/>
-    <mergeCell ref="U41:V41"/>
-    <mergeCell ref="U42:V42"/>
-    <mergeCell ref="U44:V44"/>
-    <mergeCell ref="U45:V45"/>
-    <mergeCell ref="U46:V46"/>
-    <mergeCell ref="Q30:Q37"/>
-    <mergeCell ref="U30:V30"/>
-    <mergeCell ref="U31:V31"/>
-    <mergeCell ref="U32:V32"/>
-    <mergeCell ref="U33:V33"/>
-    <mergeCell ref="U35:V35"/>
-    <mergeCell ref="U36:V36"/>
-    <mergeCell ref="U37:V37"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>